<commit_message>
added cover page to excel file
</commit_message>
<xml_diff>
--- a/Financial Data.xlsx
+++ b/Financial Data.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/138438032f8a0c27/Desktop/S23/COSC72/Final/finance-sentiment-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="564" documentId="11_F25DC773A252ABDACC1048A351984CC45BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17CDB4F7-0857-46E3-B9E7-D761A615FE56}"/>
+  <xr:revisionPtr revIDLastSave="611" documentId="11_F25DC773A252ABDACC1048A351984CC45BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CFF04BE-B24F-4C0E-B3FA-1A8600158953}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="_CIQHiddenCacheSheet" sheetId="29" state="veryHidden" r:id="rId2"/>
-    <sheet name="Summary Statistics" sheetId="18" r:id="rId3"/>
+    <sheet name="_CIQHiddenCacheSheet" sheetId="33" state="veryHidden" r:id="rId1"/>
+    <sheet name="Cover" sheetId="30" r:id="rId2"/>
+    <sheet name="Data" sheetId="1" r:id="rId3"/>
+    <sheet name="Summary Statistics" sheetId="18" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="CIQWBGuid" hidden="1">"00fd456c-f1e7-40cf-8bec-0b6061993319"</definedName>
+    <definedName name="CIQWBGuid" hidden="1">"42f12814-c4fb-4f05-80bb-96d9eed2265c"</definedName>
     <definedName name="CIQWBInfo" hidden="1">"{ ""CIQVersion"":""9.50.2716.4594"" }"</definedName>
     <definedName name="IQ_CH">110000</definedName>
     <definedName name="IQ_CQ">5000</definedName>
@@ -94,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="74">
   <si>
     <t>Ticker</t>
   </si>
@@ -243,21 +244,6 @@
     <t>FY2022 Share Price ($)</t>
   </si>
   <si>
-    <t>RVJJT0REQVRFX0JTLkZZMjAyMi4uLi5VU0QuQwEAAAAf0kwBBQAAAAk2LzMwLzIwMjIATCpqCvxk2wj2Jkxl/WTbCChDSVEuQUJULklRX1BFUklPRERBVEVfQlMuRlkyMDIwLi4uLlVTRC5DAQAAALvGAwAFAAAACjEyLzMxLzIwMjAATCpqCvxk2wj2Jkxl/WTbCChDSVEuQUJULklRX1BFUklPRERBVEVfQlMuRlkyMDIxLi4uLlVTRC5DAQAAALvGAwAFAAAACjEyLzMxLzIwMjEATCpqCvxk2wj2Jkxl/WTbCChDSVEuQUJULklRX1BFUklPRERBVEVfQlMuRlkyMDIyLi4uLlVTRC5DAQAAALvGAwAFAAAACjEyLzMxLzIwMjIATCpqCvxk2wj2Jkxl/WTbCClDSVEuQU1aTi5JUV9QRVJJT0REQVRFX0JTLkZZMjAyMC4uLi5VU0QuQwEAAAA9SQAABQAAAAoxMi8zMS8yMDIwAEwqagr8ZNsIulZMZf1k2wgpQ0lRLkFNWk4uSVFfUEVSSU9EREFURV9CUy5GWTIwMjEuLi4uVVNELkMBAAAAPUkAAAUAAAAKMTIvMzEvMjAyMQBMKmoK/GTbCLpWTGX9ZNsIKUNJUS5BTVpOLklRX1BFUklPRERBVEVfQlMuRlkyMDIyLi4uLlVTRC5DAQAAAD1JAAAFAAAACjEyLzMxLzIwMjIATCpqCvxk2wh8z0tl/WTbCClDSVEuQUJCVi5JUV9QRVJJT0REQVRFX0JTLkZZMjAyMC4uLi5VU0QuQwEAAAAKAXUIBQAAAAoxMi8zMS8yMDIwAEwqagr8ZNsIfM9LZf1k2wgpQ0lRLkFCQlYuSVFfUEVSSU9EREFURV9CUy5GWTIwMjEuLi4uVVNELkMB</t>
-  </si>
-  <si>
-    <t>AAAACgF1CAUAAAAKMTIvMzEvMjAyMQBMKmoK/GTbCHzPS2X9ZNsIKUNJUS5BQkJWLklRX1BFUklPRERBVEVfQlMuRlkyMDIyLi4uLlVTRC5DAQAAAAoBdQgFAAAACjEyLzMxLzIwMjIATCpqCvxk2wiI/0tl/WTbCClDSVEuQVZHTy5JUV9QRVJJT0REQVRFX0JTLkZZMjAyMC4uLi5VU0QuQwEAAADwtn0BBQAAAAkxMS8xLzIwMjAATCpqCvxk2wiI/0tl/WTbCClDSVEuQVZHTy5JUV9QRVJJT0REQVRFX0JTLkZZMjAyMS4uLi5VU0QuQwEAAADwtn0BBQAAAAoxMC8zMS8yMDIxAEwqagr8ZNsIiP9LZf1k2wgpQ0lRLkFWR08uSVFfUEVSSU9EREFURV9CUy5GWTIwMjIuLi4uVVNELkMBAAAA8LZ9AQUAAAAKMTAvMzAvMjAyMgBMKmoK/GTbCBOBS2X9ZNsIKUNJUS5DT1NULklRX1BFUklPRERBVEVfQlMuRlkyMDIwLi4uLlVTRC5DAQAAAJFqAQAFAAAACTgvMzAvMjAyMABMKmoK/GTbCBOBS2X9ZNsIKUNJUS5DT1NULklRX1BFUklPRERBVEVfQlMuRlkyMDIxLi4uLlVTRC5DAQAAAJFqAQAFAAAACTgvMjkvMjAyMQBMKmoK/GTbCF+oS2X9ZNsIKUNJUS5DT1NULklRX1BFUklPRERBVEVfQlMuRlkyMDIyLi4uLlVTRC5DAQAAAJFqAQAFAAAACTgvMjgvMjAyMgBMKmoK/GTbCF+oS2X9ZNsIKUNJUS5HT09HLklRX1BFUklPRERBVEVfQlMuRlkyMDIwLi4uLlVTRC5DAQAAAKhxAAAFAAAACjEyLzMxLzIwMjAATCpqCvxk</t>
-  </si>
-  <si>
-    <t>2whfqEtl/WTbCClDSVEuR09PRy5JUV9QRVJJT0REQVRFX0JTLkZZMjAyMS4uLi5VU0QuQwEAAACocQAABQAAAAoxMi8zMS8yMDIxAEwqagr8ZNsIX6hLZf1k2wgpQ0lRLkdPT0cuSVFfUEVSSU9EREFURV9CUy5GWTIwMjIuLi4uVVNELkMBAAAAqHEAAAUAAAAKMTIvMzEvMjAyMgBMKmoK/GTbCM4oS2X9ZNsIKENJUS5CQUMuSVFfUEVSSU9EREFURV9CUy5GWTIwMjAuLi4uVVNELkMBAAAAaUoAAAUAAAAKMTIvMzEvMjAyMABMKmoK/GTbCChUS2X9ZNsIKENJUS5CQUMuSVFfUEVSSU9EREFURV9CUy5GWTIwMjEuLi4uVVNELkMBAAAAaUoAAAUAAAAKMTIvMzEvMjAyMQBMKmoK/GTbCChUS2X9ZNsIKENJUS5CQUMuSVFfUEVSSU9EREFURV9CUy5GWTIwMjIuLi4uVVNELkMBAAAAaUoAAAUAAAAKMTIvMzEvMjAyMgBMKmoK/GTbCChUS2X9ZNsIKENJUS5NUksuSVFfUEVSSU9EREFURV9CUy5GWTIwMjAuLi4uVVNELkMBAAAA9mYEAAUAAAAKMTIvMzEvMjAyMABMKmoK/GTbCChUS2X9ZNsIKENJUS5NUksuSVFfUEVSSU9EREFURV9CUy5GWTIwMjEuLi4uVVNELkMBAAAA9mYEAAUAAAAKMTIvMzEvMjAyMQBMKmoK/GTbCBOBS2X9ZNsIKENJUS5NUksuSVFfUEVSSU9EREFURV9CUy5GWTIwMjIuLi4uVVNELkMBAAAA9mYEAAUAAAAKMTIvMzEvMjAyMgBMKmoK/GTbCIEBS2X9ZNsIKUNJUS5NU0ZULklRX1BFUklPRERB</t>
-  </si>
-  <si>
-    <t>VEVfQlMuRlkyMDIwLi4uLlVTRC5DAQAAAEtVAAAFAAAACTYvMzAvMjAyMABMKmoK/GTbCIEBS2X9ZNsIKUNJUS5NU0ZULklRX1BFUklPRERBVEVfQlMuRlkyMDIxLi4uLlVTRC5DAQAAAEtVAAAFAAAACTYvMzAvMjAyMQBMKmoK/GTbCIEBS2X9ZNsIKUNJUS5NU0ZULklRX1BFUklPRERBVEVfQlMuRlkyMDIyLi4uLlVTRC5DAQAAAEtVAAAFAAAACTYvMzAvMjAyMgBMKmoK/GTbCIEBS2X9ZNsIJ0NJUS5LTy5JUV9QRVJJT0REQVRFX0JTLkZZMjAyMC4uLi5VU0QuQwEAAAASaAAABQAAAAoxMi8zMS8yMDIwAEwqagr8ZNsIzihLZf1k2wgnQ0lRLktPLklRX1BFUklPRERBVEVfQlMuRlkyMDIxLi4uLlVTRC5DAQAAABJoAAAFAAAACjEyLzMxLzIwMjEATCpqCvxk2wjOKEtl/WTbCCdDSVEuS08uSVFfUEVSSU9EREFURV9CUy5GWTIwMjIuLi4uVVNELkMBAAAAEmgAAAUAAAAKMTIvMzEvMjAyMgBMKmoK/GTbCGCfSmX9ZNsIKENJUS5NQ0QuSVFfUEVSSU9EREFURV9CUy5GWTIwMjAuLi4uVVNELkMBAAAA4CACAAUAAAAKMTIvMzEvMjAyMABMKmoK/GTbCGCfSmX9ZNsIKENJUS5NQ0QuSVFfUEVSSU9EREFURV9CUy5GWTIwMjEuLi4uVVNELkMBAAAA4CACAAUAAAAKMTIvMzEvMjAyMQBMKmoK/GTbCNvGSmX9ZNsIKENJUS5NQ0QuSVFfUEVSSU9EREFURV9CUy5GWTIwMjIuLi4uVVNELkMBAAAA4CACAAUAAAAKMTIv</t>
-  </si>
-  <si>
-    <t>MzEvMjAyMgBMKmoK/GTbCNvGSmX9ZNsIKUNJUS5NRVRBLklRX1BFUklPRERBVEVfQlMuRlkyMDIwLi4uLlVTRC5DAQAAABfbPAEFAAAACjEyLzMxLzIwMjAATCpqCvxk2wjbxkpl/WTbCClDSVEuTUVUQS5JUV9QRVJJT0REQVRFX0JTLkZZMjAyMS4uLi5VU0QuQwEAAAAX2zwBBQAAAAoxMi8zMS8yMDIxAEwqagr8ZNsIxe1KZf1k2wgpQ0lRLk1FVEEuSVFfUEVSSU9EREFURV9CUy5GWTIwMjIuLi4uVVNELkMBAAAAF9s8AQUAAAAKMTIvMzEvMjAyMgBMKmoK/GTbCBFoSmX9ZNsIJ0NJUS5IRC5JUV9QRVJJT0REQVRFX0JTLkZZMjAyMC4uLi5VU0QuQwEAAACXQAQABQAAAAgyLzIvMjAyMABMKmoK/GTbCBFoSmX9ZNsIJ0NJUS5IRC5JUV9QRVJJT0REQVRFX0JTLkZZMjAyMS4uLi5VU0QuQwEAAACXQAQABQAAAAkxLzMxLzIwMjEATCpqCvxk2wgRaEpl/WTbCCdDSVEuSEQuSVFfUEVSSU9EREFURV9CUy5GWTIwMjIuLi4uVVNELkMBAAAAl0AEAAUAAAAJMS8zMC8yMDIyAEwqagr8ZNsIEWhKZf1k2wgoQ0lRLkpQTS5JUV9QRVJJT0REQVRFX0JTLkZZMjAyMC4uLi5VU0QuQwEAAABYDQoABQAAAAoxMi8zMS8yMDIwAEwqagr8ZNsIEWhKZf1k2wgoQ0lRLkpQTS5JUV9QRVJJT0REQVRFX0JTLkZZMjAyMS4uLi5VU0QuQwEAAABYDQoABQAAAAoxMi8zMS8yMDIxAEwqagr8ZNsIYJ9KZf1k2wgoQ0lRLkpQTS5JUV9Q</t>
-  </si>
-  <si>
     <t>TABLE I</t>
   </si>
   <si>
@@ -285,97 +271,52 @@
     <t>Median</t>
   </si>
   <si>
-    <t>BAABTAVMT0NBTAFI/////wFQRwEAAClDSVEuQUFQTC5JUV9QRVJJT0REQVRFX0JTLkZZMjAyMC4uLi5VU0QuQwEAAABpYQAABQAAAAk5LzI2LzIwMjAATCpqCvxk2wi6Vkxl/WTbCClDSVEuQUFQTC5JUV9QRVJJT0REQVRFX0JTLkZZMjAyMS4uLi5VU0QuQwEAAABpYQAABQAAAAk5LzI1LzIwMjEATCpqCvxk2wgGfkxl/WTbCClDSVEuQUFQTC5JUV9QRVJJT0REQVRFX0JTLkZZMjAyMi4uLi5VU0QuQwEAAABpYQAABQAAAAk5LzI0LzIwMjIATCpqCvxk2wgRk0xl/WTbCChDSVEuQ1ZYLklRX1BFUklPRERBVEVfQlMuRlkyMDIwLi4uLlVTRC5DAQAAAMqAAQAFAAAACjEyLzMxLzIwMjAATCpqCvxk2wgRk0xl/WTbCChDSVEuQ1ZYLklRX1BFUklPRERBVEVfQlMuRlkyMDIxLi4uLlVTRC5DAQAAAMqAAQAFAAAACjEyLzMxLzIwMjEATCpqCvxk2wjvukxl/WTbCChDSVEuQ1ZYLklRX1BFUklPRERBVEVfQlMuRlkyMDIyLi4uLlVTRC5DAQAAAMqAAQAFAAAACjEyLzMxLzIwMjIATCpqCvxk2wjvukxl/WTbCChDSVEuQlJLLklRX1BFUklPRERBVEVfQlMuRlkyMDIwLi4uLlVTRC5DAQAAAB/STAEFAAAACTYvMzAvMjAyMABMKmoK/GTbCO+6TGX9ZNsIKENJUS5CUksuSVFfUEVSSU9EREFURV9CUy5GWTIwMjEuLi4uVVNELkMBAAAAH9JMAQUAAAAJNi8zMC8yMDIxAEwqagr8ZNsI9iZMZf1k2wgoQ0lRLkJSSy5JUV9Q</t>
-  </si>
-  <si>
-    <t>RVJJT0REQVRFX0JTLkZZMjAyMi4uLi5VU0QuQwEAAABYDQoABQAAAAoxMi8zMS8yMDIyAEwqagr8ZNsI1BFKZf1k2wgoQ0lRLkpOSi5JUV9QRVJJT0REQVRFX0JTLkZZMjAyMC4uLi5VU0QuQwEAAACdIQIABQAAAAgxLzMvMjAyMQBMKmoK/GTbCNQRSmX9ZNsIKENJUS5KTkouSVFfUEVSSU9EREFURV9CUy5GWTIwMjEuLi4uVVNELkMBAAAAnSECAAUAAAAIMS8yLzIwMjIATCpqCvxk2wjUEUpl/WTbCClDSVEuTlZEQS5JUV9QRVJJT0REQVRFX0JTLkZZMjAyMS4uLi5VU0QuQwEAAAAzfgAABQAAAAkxLzMxLzIwMjEATCpqCvxk2wix1kll/WTbCChDSVEuUEZFLklRX1BFUklPRERBVEVfQlMuRlkyMDIyLi4uLlVTRC5DAQAAAN55AgAFAAAACjEyLzMxLzIwMjIATCpqCvxk2wjRSEll/WTbCCZDSVEuVi5JUV9QRVJJT0REQVRFX0JTLkZZMjAyMC4uLi5VU0QuQwEAAABLf0QCBQAAAAk5LzMwLzIwMjAATCpqCvxk2wjcZUll/WTbCCZDSVEuVi5JUV9QRVJJT0REQVRFX0JTLkZZMjAyMS4uLi5VU0QuQwEAAABLf0QCBQAAAAk5LzMwLzIwMjEATCpqCvxk2wgMdEll/WTbCChDSVEuVU5ILklRX1BFUklPRERBVEVfQlMuRlkyMDIwLi4uLlVTRC5DAQAAAOGYAQAFAAAACjEyLzMxLzIwMjAATCpqCvxk2wgH9Uhl/WTbCChDSVEuVU5ILklRX1BFUklPRERBVEVfQlMuRlkyMDIxLi4uLlVTRC5DAQAAAOGYAQAFAAAACjEy</t>
-  </si>
-  <si>
-    <t>LzMxLzIwMjEATCpqCvxk2wiJLEll/WTbCClDSVEuQUFQTC5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLjkvMjYvMjAyMAEAAABpYQAABQAAAAoxMC8yOC8yMDIyAGUFTefwZNsIBn5MZf1k2wgrQ0lRLkFBUEwuSVFfRklMSU5HREFURV9CUy5JUV9GWS0xLjkvMjYvMjAyMAEAAABpYQAABQAAAAoxMC8yOS8yMDIxADReuf/7ZNsIBn5MZf1k2wgoQ0lRLkpOSi5JUV9QRVJJT0REQVRFX0JTLkZZMjAyMi4uLi5VU0QuQwEAAACdIQIABQAAAAgxLzEvMjAyMwBMKmoK/GTbCNQRSmX9ZNsIKENJUS5MTFkuSVFfUEVSSU9EREFURV9CUy5GWTIwMjAuLi4uVVNELkMBAAAAG1sEAAUAAAAKMTIvMzEvMjAyMABMKmoK/GTbCNQRSmX9ZNsIKENJUS5MTFkuSVFfUEVSSU9EREFURV9CUy5GWTIwMjEuLi4uVVNELkMBAAAAG1sEAAUAAAAKMTIvMzEvMjAyMQBMKmoK/GTbCIJASmX9ZNsIKENJUS5MTFkuSVFfUEVSSU9EREFURV9CUy5GWTIwMjIuLi4uVVNELkMBAAAAG1sEAAUAAAAKMTIvMzEvMjAyMgBMKmoK/GTbCNLCSWX9ZNsIKUNJUS5OVkRBLklRX1BFUklPRERBVEVfQlMuRlkyMDIwLi4uLlVTRC5DAQAAADN+AAAFAAAACTEvMjYvMjAyMABMKmoK/GTbCLHWSWX9ZNsIKUNJUS5OVkRBLklRX1BFUklPRERBVEVfQlMuRlkyMDIyLi4uLlVTRC5DAQAAADN+AAAFAAAACTEvMzAvMjAyMgBMKmoK/GTbCHjqSWX9ZNsIKUNJUS5U</t>
-  </si>
-  <si>
-    <t>U0xBLklRX1BFUklPRERBVEVfQlMuRlkyMDIwLi4uLlVTRC5DAQAAABDGogEFAAAACjEyLzMxLzIwMjAATCpqCvxk2wh46kll/WTbCClDSVEuVFNMQS5JUV9QRVJJT0REQVRFX0JTLkZZMjAyMS4uLi5VU0QuQwEAAAAQxqIBBQAAAAoxMi8zMS8yMDIxAEwqagr8ZNsIeOpJZf1k2wgpQ0lRLlRTTEEuSVFfUEVSSU9EREFURV9CUy5GWTIwMjIuLi4uVVNELkMBAAAAEMaiAQUAAAAKMTIvMzEvMjAyMgBMKmoK/GTbCAx0SWX9ZNsIJ0NJUS5QRy5JUV9QRVJJT0REQVRFX0JTLkZZMjAyMC4uLi5VU0QuQwEAAAAwggAABQAAAAk2LzMwLzIwMjAATCpqCvxk2wgMdEll/WTbCCdDSVEuUEcuSVFfUEVSSU9EREFURV9CUy5GWTIwMjEuLi4uVVNELkMBAAAAMIIAAAUAAAAJNi8zMC8yMDIxAEwqagr8ZNsIDHRJZf1k2wgnQ0lRLlBHLklRX1BFUklPRERBVEVfQlMuRlkyMDIyLi4uLlVTRC5DAQAAADCCAAAFAAAACTYvMzAvMjAyMgBMKmoK/GTbCGObSWX9ZNsIKENJUS5YT00uSVFfUEVSSU9EREFURV9CUy5GWTIwMjAuLi4uVVNELkMBAAAAQjMGAAUAAAAKMTIvMzEvMjAyMABMKmoK/GTbCGObSWX9ZNsIKENJUS5YT00uSVFfUEVSSU9EREFURV9CUy5GWTIwMjEuLi4uVVNELkMBAAAAQjMGAAUAAAAKMTIvMzEvMjAyMQBMKmoK/GTbCGObSWX9ZNsIKENJUS5YT00uSVFfUEVSSU9EREFURV9CUy5GWTIwMjIuLi4uVVNELkMB</t>
-  </si>
-  <si>
-    <t>AAAAQjMGAAUAAAAKMTIvMzEvMjAyMgBMKmoK/GTbCIksSWX9ZNsIKENJUS5QRkUuSVFfUEVSSU9EREFURV9CUy5GWTIwMjAuLi4uVVNELkMBAAAA3nkCAAUAAAAKMTIvMzEvMjAyMABMKmoK/GTbCIksSWX9ZNsIKENJUS5QRkUuSVFfUEVSSU9EREFURV9CUy5GWTIwMjEuLi4uVVNELkMBAAAA3nkCAAUAAAAKMTIvMzEvMjAyMQBMKmoK/GTbCNFISWX9ZNsIK0NJUS5BQVBMLklRX0ZJTElOR0RBVEVfQlMuSVFfRlktMi45LzI2LzIwMjABAAAAaWEAAAUAAAAKMTAvMzAvMjAyMABO8rVY/GTbCLpWTGX9ZNsIK0NJUS5DVlguSVFfRklMSU5HREFURV9CUy5JUV9GWS0yLjEyLzMxLzIwMjABAAAAyoABAAUAAAAJMi8yNS8yMDIxAHD7IIv8ZNsIEZNMZf1k2wgrQ0lRLkNWWC5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLTEuMTIvMzEvMjAyMAEAAADKgAEABQAAAAkyLzI0LzIwMjIAcPsgi/xk2wgRk0xl/WTbCClDSVEuQ1ZYLklRX0ZJTElOR0RBVEVfQlMuSVFfRlkuMTIvMzEvMjAyMAEAAADKgAEABQAAAAkyLzIzLzIwMjMAcPsgi/xk2wgRk0xl/WTbCCpDSVEuQlJLLklRX0ZJTElOR0RBVEVfQlMuSVFfRlktMi42LzMwLzIwMjABAAAAH9JMAQUAAAAJOS8yOC8yMDE5AHD7IIv8ZNsI77pMZf1k2wgqQ0lRLkJSSy5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLTEuNi8zMC8yMDIwAQAAAB/STAEFAAAACTkvMjYvMjAyMABw</t>
-  </si>
-  <si>
-    <t>+yCL/GTbCO+6TGX9ZNsIKENJUS5CUksuSVFfRklMSU5HREFURV9CUy5JUV9GWS42LzMwLzIwMjABAAAAH9JMAQUAAAAJOS8yNy8yMDIxAHD7IIv8ZNsI77pMZf1k2wgrQ0lRLkFCVC5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLTIuMTIvMzEvMjAyMAEAAAC7xgMABQAAAAkyLzE5LzIwMjEAcPsgi/xk2wj2Jkxl/WTbCCtDSVEuQUJULklRX0ZJTElOR0RBVEVfQlMuSVFfRlktMS4xMi8zMS8yMDIwAQAAALvGAwAFAAAACTIvMTgvMjAyMgBw+yCL/GTbCPYmTGX9ZNsIKUNJUS5BQlQuSVFfRklMSU5HREFURV9CUy5JUV9GWS4xMi8zMS8yMDIwAQAAALvGAwAFAAAACTIvMTcvMjAyMwBw+yCL/GTbCPYmTGX9ZNsILENJUS5BTVpOLklRX0ZJTElOR0RBVEVfQlMuSVFfRlktMi4xMi8zMS8yMDIwAQAAAD1JAAAFAAAACDIvMy8yMDIxAHD7IIv8ZNsIulZMZf1k2wgsQ0lRLkFNWk4uSVFfRklMSU5HREFURV9CUy5JUV9GWS0xLjEyLzMxLzIwMjABAAAAPUkAAAUAAAAIMi80LzIwMjIAcPsgi/xk2wi6Vkxl/WTbCCpDSVEuQU1aTi5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLjEyLzMxLzIwMjABAAAAPUkAAAUAAAAIMi8zLzIwMjMAcPsgi/xk2wi6Vkxl/WTbCCxDSVEuQUJCVi5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLTIuMTIvMzEvMjAyMAEAAAAKAXUIBQAAAAkyLzE5LzIwMjEAcPsgi/xk2wh8z0tl/WTbCCxDSVEuQUJC</t>
-  </si>
-  <si>
-    <t>Vi5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLTEuMTIvMzEvMjAyMAEAAAAKAXUIBQAAAAkyLzE4LzIwMjIAcPsgi/xk2wh8z0tl/WTbCCpDSVEuQUJCVi5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLjEyLzMxLzIwMjABAAAACgF1CAUAAAAJMi8xNy8yMDIzAHD7IIv8ZNsIfM9LZf1k2wgrQ0lRLkFWR08uSVFfRklMSU5HREFURV9CUy5JUV9GWS0yLjExLzEvMjAyMAEAAADwtn0BBQAAAAoxMi8xOC8yMDIwAHD7IIv8ZNsIiP9LZf1k2wgrQ0lRLkFWR08uSVFfRklMSU5HREFURV9CUy5JUV9GWS0xLjExLzEvMjAyMAEAAADwtn0BBQAAAAoxMi8xNy8yMDIxAHD7IIv8ZNsIiP9LZf1k2wgpQ0lRLkFWR08uSVFfRklMSU5HREFURV9CUy5JUV9GWS4xMS8xLzIwMjABAAAA8LZ9AQUAAAAKMTIvMTYvMjAyMgBw+yCL/GTbCIj/S2X9ZNsIK0NJUS5DT1NULklRX0ZJTElOR0RBVEVfQlMuSVFfRlktMi44LzMwLzIwMjABAAAAkWoBAAUAAAAJMTAvNy8yMDIwAHD7IIv8ZNsIE4FLZf1k2wgrQ0lRLkNPU1QuSVFfRklMSU5HREFURV9CUy5JUV9GWS0xLjgvMzAvMjAyMAEAAACRagEABQAAAAkxMC82LzIwMjEAcPsgi/xk2wgTgUtl/WTbCClDSVEuQ09TVC5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLjgvMzAvMjAyMAEAAACRagEABQAAAAkxMC81LzIwMjIAcPsgi/xk2wgTgUtl/WTbCCxDSVEuR09PRy5JUV9GSUxJTkdEQVRFX0JT</t>
-  </si>
-  <si>
-    <t>LklRX0ZZLTIuMTIvMzEvMjAyMAEAAACocQAABQAAAAgyLzMvMjAyMQBw+yCL/GTbCF+oS2X9ZNsILENJUS5HT09HLklRX0ZJTElOR0RBVEVfQlMuSVFfRlktMS4xMi8zMS8yMDIwAQAAAKhxAAAFAAAACDIvMi8yMDIyAHD7IIv8ZNsIX6hLZf1k2wgqQ0lRLkdPT0cuSVFfRklMSU5HREFURV9CUy5JUV9GWS4xMi8zMS8yMDIwAQAAAKhxAAAFAAAACDIvMy8yMDIzAHD7IIv8ZNsIX6hLZf1k2wgrQ0lRLkJBQy5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLTIuMTIvMzEvMjAyMAEAAABpSgAABQAAAAkyLzI0LzIwMjEAcPsgi/xk2wgoVEtl/WTbCCtDSVEuQkFDLklRX0ZJTElOR0RBVEVfQlMuSVFfRlktMS4xMi8zMS8yMDIwAQAAAGlKAAAFAAAACTIvMjIvMjAyMgBw+yCL/GTbCChUS2X9ZNsIKUNJUS5CQUMuSVFfRklMSU5HREFURV9CUy5JUV9GWS4xMi8zMS8yMDIwAQAAAGlKAAAFAAAACTIvMjIvMjAyMwBw+yCL/GTbCChUS2X9ZNsIK0NJUS5NUksuSVFfRklMSU5HREFURV9CUy5JUV9GWS0yLjEyLzMxLzIwMjABAAAA9mYEAAUAAAAJMi8yNS8yMDIxAHD7IIv8ZNsIE4FLZf1k2wgrQ0lRLk1SSy5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLTEuMTIvMzEvMjAyMAEAAAD2ZgQABQAAAAkyLzI1LzIwMjIAcPsgi/xk2wgTgUtl/WTbCClDSVEuTVJLLklRX0ZJTElOR0RBVEVfQlMuSVFfRlkuMTIvMzEvMjAyMAEAAAD2</t>
-  </si>
-  <si>
-    <t>ZgQABQAAAAkyLzI0LzIwMjMAcPsgi/xk2wgoVEtl/WTbCCtDSVEuTVNGVC5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLTIuNi8zMC8yMDIwAQAAAEtVAAAFAAAACTcvMzEvMjAyMABw+yCL/GTbCIEBS2X9ZNsIK0NJUS5NU0ZULklRX0ZJTElOR0RBVEVfQlMuSVFfRlktMS42LzMwLzIwMjABAAAAS1UAAAUAAAAJNy8yOS8yMDIxAHD7IIv8ZNsIgQFLZf1k2wgpQ0lRLk1TRlQuSVFfRklMSU5HREFURV9CUy5JUV9GWS42LzMwLzIwMjABAAAAS1UAAAUAAAAJNy8yOC8yMDIyAHD7IIv8ZNsIgQFLZf1k2wgqQ0lRLktPLklRX0ZJTElOR0RBVEVfQlMuSVFfRlktMi4xMi8zMS8yMDIwAQAAABJoAAAFAAAACTIvMjUvMjAyMQBw+yCL/GTbCM4oS2X9ZNsIKkNJUS5LTy5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLTEuMTIvMzEvMjAyMAEAAAASaAAABQAAAAkyLzIyLzIwMjIAcPsgi/xk2wjOKEtl/WTbCChDSVEuS08uSVFfRklMSU5HREFURV9CUy5JUV9GWS4xMi8zMS8yMDIwAQAAABJoAAAFAAAACTIvMjEvMjAyMwBw+yCL/GTbCM4oS2X9ZNsIK0NJUS5NQ0QuSVFfRklMSU5HREFURV9CUy5JUV9GWS0yLjEyLzMxLzIwMjABAAAA4CACAAUAAAAJMi8yMy8yMDIxAHD7IIv8ZNsIYJ9KZf1k2wgrQ0lRLk1DRC5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLTEuMTIvMzEvMjAyMAEAAADgIAIABQAAAAkyLzI0LzIwMjIAcPsgi/xk</t>
-  </si>
-  <si>
-    <t>2whgn0pl/WTbCClDSVEuTUNELklRX0ZJTElOR0RBVEVfQlMuSVFfRlkuMTIvMzEvMjAyMAEAAADgIAIABQAAAAkyLzI0LzIwMjMAcPsgi/xk2wjbxkpl/WTbCCxDSVEuTUVUQS5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLTIuMTIvMzEvMjAyMAEAAAAX2zwBBQAAAAkxLzI4LzIwMjEAcPsgi/xk2wjF7Upl/WTbCCxDSVEuTUVUQS5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLTEuMTIvMzEvMjAyMAEAAAAX2zwBBQAAAAgyLzMvMjAyMgBw+yCL/GTbCNvGSmX9ZNsIKkNJUS5NRVRBLklRX0ZJTElOR0RBVEVfQlMuSVFfRlkuMTIvMzEvMjAyMAEAAAAX2zwBBQAAAAgyLzIvMjAyMwBw+yCL/GTbCNvGSmX9ZNsIKENJUS5IRC5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLTIuMi8yLzIwMjABAAAAl0AEAAUAAAAJMy8yNS8yMDIwAHD7IIv8ZNsIEWhKZf1k2wgoQ0lRLkhELklRX0ZJTElOR0RBVEVfQlMuSVFfRlktMS4yLzIvMjAyMAEAAACXQAQABQAAAAkzLzI0LzIwMjEAcPsgi/xk2wgRaEpl/WTbCCZDSVEuSEQuSVFfRklMSU5HREFURV9CUy5JUV9GWS4yLzIvMjAyMAEAAACXQAQABQAAAAkzLzIzLzIwMjIAcPsgi/xk2wgRaEpl/WTbCCtDSVEuSlBNLklRX0ZJTElOR0RBVEVfQlMuSVFfRlktMi4xMi8zMS8yMDIwAQAAAFgNCgAFAAAACTIvMjMvMjAyMQBw+yCL/GTbCGCfSmX9ZNsIK0NJUS5KUE0uSVFfRklMSU5HREFU</t>
-  </si>
-  <si>
-    <t>RV9CUy5JUV9GWS0xLjEyLzMxLzIwMjABAAAAWA0KAAUAAAAJMi8yMi8yMDIyAHD7IIv8ZNsIYJ9KZf1k2wgpQ0lRLkpQTS5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLjEyLzMxLzIwMjABAAAAWA0KAAUAAAAJMi8yMS8yMDIzAHD7IIv8ZNsIEWhKZf1k2wgpQ0lRLkpOSi5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLTIuMS8zLzIwMjEBAAAAnSECAAUAAAAJMi8yMi8yMDIxAHD7IIv8ZNsI1BFKZf1k2wgpQ0lRLkpOSi5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLTEuMS8zLzIwMjEBAAAAnSECAAUAAAAJMi8xNy8yMDIyAHD7IIv8ZNsI1BFKZf1k2wgnQ0lRLkpOSi5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLjEvMy8yMDIxAQAAAJ0hAgAFAAAACTIvMTYvMjAyMwBw+yCL/GTbCNQRSmX9ZNsIK0NJUS5MTFkuSVFfRklMSU5HREFURV9CUy5JUV9GWS0yLjEyLzMxLzIwMjABAAAAG1sEAAUAAAAJMi8xNy8yMDIxAHD7IIv8ZNsIgkBKZf1k2wgrQ0lRLkxMWS5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLTEuMTIvMzEvMjAyMAEAAAAbWwQABQAAAAkyLzIzLzIwMjIAcPsgi/xk2wiCQEpl/WTbCClDSVEuTExZLklRX0ZJTElOR0RBVEVfQlMuSVFfRlkuMTIvMzEvMjAyMAEAAAAbWwQABQAAAAkyLzIyLzIwMjMAcPsgi/xk2wiCQEpl/WTbCCtDSVEuTlZEQS5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLTIuMS8yNi8yMDIwAQAAADN+</t>
-  </si>
-  <si>
-    <t>AAAFAAAACTIvMjAvMjAyMABw+yCL/GTbCLHWSWX9ZNsIK0NJUS5OVkRBLklRX0ZJTElOR0RBVEVfQlMuSVFfRlktMS4xLzI2LzIwMjABAAAAM34AAAUAAAAJMi8yNi8yMDIxAHD7IIv8ZNsIsdZJZf1k2wgpQ0lRLk5WREEuSVFfRklMSU5HREFURV9CUy5JUV9GWS4xLzI2LzIwMjABAAAAM34AAAUAAAAJMy8xOC8yMDIyAHD7IIv8ZNsIsdZJZf1k2wgsQ0lRLlRTTEEuSVFfRklMSU5HREFURV9CUy5JUV9GWS0yLjEyLzMxLzIwMjABAAAAEMaiAQUAAAAIMi84LzIwMjEAcPsgi/xk2wh46kll/WTbCCxDSVEuVFNMQS5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLTEuMTIvMzEvMjAyMAEAAAAQxqIBBQAAAAgyLzcvMjAyMgBw+yCL/GTbCHjqSWX9ZNsIKkNJUS5UU0xBLklRX0ZJTElOR0RBVEVfQlMuSVFfRlkuMTIvMzEvMjAyMAEAAAAQxqIBBQAAAAkxLzMxLzIwMjMAcPsgi/xk2wh46kll/WTbCClDSVEuUEcuSVFfRklMSU5HREFURV9CUy5JUV9GWS0yLjYvMzAvMjAyMAEAAAAwggAABQAAAAk4LzEwLzIwMjAAcPsgi/xk2wgMdEll/WTbCClDSVEuUEcuSVFfRklMSU5HREFURV9CUy5JUV9GWS0xLjYvMzAvMjAyMAEAAAAwggAABQAAAAg4LzYvMjAyMQBw+yCL/GTbCAx0SWX9ZNsIJ0NJUS5QRy5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLjYvMzAvMjAyMAEAAAAwggAABQAAAAg4LzUvMjAyMgBw+yCL/GTbCAx0SWX9</t>
-  </si>
-  <si>
-    <t>ZNsIK0NJUS5YT00uSVFfRklMSU5HREFURV9CUy5JUV9GWS0yLjEyLzMxLzIwMjABAAAAQjMGAAUAAAAJMi8yNC8yMDIxAHD7IIv8ZNsIY5tJZf1k2wgrQ0lRLlhPTS5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLTEuMTIvMzEvMjAyMAEAAABCMwYABQAAAAkyLzIzLzIwMjIAcPsgi/xk2whjm0ll/WTbCClDSVEuWE9NLklRX0ZJTElOR0RBVEVfQlMuSVFfRlkuMTIvMzEvMjAyMAEAAABCMwYABQAAAAkyLzIyLzIwMjMAcPsgi/xk2whjm0ll/WTbCCtDSVEuUEZFLklRX0ZJTElOR0RBVEVfQlMuSVFfRlktMi4xMi8zMS8yMDIwAQAAAN55AgAFAAAACTIvMjUvMjAyMQBw+yCL/GTbCNFISWX9ZNsIK0NJUS5QRkUuSVFfRklMSU5HREFURV9CUy5JUV9GWS0xLjEyLzMxLzIwMjABAAAA3nkCAAUAAAAJMi8yNC8yMDIyAHD7IIv8ZNsI0UhJZf1k2wgpQ0lRLlBGRS5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLjEyLzMxLzIwMjABAAAA3nkCAAUAAAAJMi8yMy8yMDIzAHD7IIv8ZNsI0UhJZf1k2wgoQ0lRLlYuSVFfRklMSU5HREFURV9CUy5JUV9GWS0yLjkvMzAvMjAyMAEAAABLf0QCBQAAAAoxMS8xOS8yMDIwAHD7IIv8ZNsIDHRJZf1k2wgoQ0lRLlYuSVFfRklMSU5HREFURV9CUy5JUV9GWS0xLjkvMzAvMjAyMAEAAABLf0QCBQAAAAoxMS8xOC8yMDIxAHD7IIv8ZNsI3GVJZf1k2wgmQ0lRLlYuSVFfRklMSU5HREFURV9C</t>
-  </si>
-  <si>
-    <t>Uy5JUV9GWS45LzMwLzIwMjABAAAAS39EAgUAAAAKMTEvMTYvMjAyMgBw+yCL/GTbCNxlSWX9ZNsIK0NJUS5QRVAuSVFfRklMSU5HREFURV9CUy5JUV9GWS0yLjEyLzI2LzIwMjABAAAAVoAAAAUAAAAJMi8xMS8yMDIxAHD7IIv8ZNsIB/VIZf1k2wgrQ0lRLlBFUC5JUV9GSUxJTkdEQVRFX0JTLklRX0ZZLTEuMTIvMjYvMjAyMAEAAABWgAAABQAAAAkyLzEwLzIwMjIAcPsgi/xk2wgH9Uhl/WTbCClDSVEuUEVQLklRX0ZJTElOR0RBVEVfQlMuSVFfRlkuMTIvMjYvMjAyMAEAAABWgAAABQAAAAgyLzkvMjAyMwBw+yCL/GTbCAf1SGX9ZNsIK0NJUS5VTkguSVFfRklMSU5HREFURV9CUy5JUV9GWS0yLjEyLzMxLzIwMjABAAAA4ZgBAAUAAAAIMy8xLzIwMjEAcPsgi/xk2wgH9Uhl/WTbCCtDSVEuVU5ILklRX0ZJTElOR0RBVEVfQlMuSVFfRlktMS4xMi8zMS8yMDIwAQAAAOGYAQAFAAAACTIvMTUvMjAyMgBw+yCL/GTbCAf1SGX9ZNsIKUNJUS5VTkguSVFfRklMSU5HREFURV9CUy5JUV9GWS4xMi8zMS8yMDIwAQAAAOGYAQAFAAAACTIvMjQvMjAyMwBw+yCL/GTbCAf1SGX9ZNsIH0NJUS5BQVBMLklRX0xBU1RTQUxFUFJJQ0UuNDQxMzMBAAAAaWEAAAIAAAAGMTE1LjMyAJ4yiRH9ZNsIEZNMZf1k2wgeQ0lRLkNWWC5JUV9MQVNUU0FMRVBSSUNFLjQ0MjUxAQAAAMqAAQACAAAABjEwMy4zMQCeMokR/WTbCO+6TGX9</t>
-  </si>
-  <si>
-    <t>ZNsIHkNJUS5CUksuSVFfTEFTVFNBTEVQUklDRS40MzczNQEAAAAf0kwBAgAAAAYxOS45MjUAnjKJEf1k2wjvukxl/WTbCB5DSVEuQUJULklRX0xBU1RTQUxFUFJJQ0UuNDQyNDUBAAAAu8YDAAIAAAAGMTI1LjQxAJ4yiRH9ZNsI9iZMZf1k2wgfQ0lRLkFNWk4uSVFfTEFTVFNBTEVQUklDRS40NDIyOQEAAAA9SQAAAgAAAAMxNjkAnjKJEf1k2wi6Vkxl/WTbCB9DSVEuQUJCVi5JUV9MQVNUU0FMRVBSSUNFLjQ0MjQ1AQAAAAoBdQgCAAAABjEwNi4wNgCeMokR/WTbCHzPS2X9ZNsIH0NJUS5BVkdPLklRX0xBU1RTQUxFUFJJQ0UuNDQxODIBAAAA8LZ9AQIAAAAFNDI2LjEAnjKJEf1k2wj2Jkxl/WTbCB9DSVEuQ09TVC5JUV9MQVNUU0FMRVBSSUNFLjQ0MTEwAQAAAJFqAQACAAAABjM1OC4zNQCeMokR/WTbCF+oS2X9ZNsIH0NJUS5HT09HLklRX0xBU1RTQUxFUFJJQ0UuNDQyMjkBAAAAqHEAAAIAAAAHOTYuMzc1NQCeMokR/WTbCHzPS2X9ZNsIHkNJUS5CQUMuSVFfTEFTVFNBTEVQUklDRS40NDI1MAEAAABpSgAAAgAAAAUzNS41MgCeMokR/WTbCChUS2X9ZNsIHkNJUS5NUksuSVFfTEFTVFNBTEVQUklDRS40NDI1MQEAAAD2ZgQAAgAAAAU3NC41NwCeMokR/WTbCBOBS2X9ZNsIH0NJUS5NU0ZULklRX0xBU1RTQUxFUFJJQ0UuNDQwNDIBAAAAS1UAAAIAAAAFMjAzLjkAnjKJEf1k2wiBAUtl/WTbCB1DSVEuS08u</t>
-  </si>
-  <si>
-    <t>SVFfTEFTVFNBTEVQUklDRS40NDI1MQEAAAASaAAAAgAAAAU1MC43MQCeMokR/WTbCM4oS2X9ZNsIHkNJUS5NQ0QuSVFfTEFTVFNBTEVQUklDRS40NDI0OQEAAADgIAIAAgAAAAYyMTIuMDYAnjKJEf1k2wjbxkpl/WTbCB9DSVEuTUVUQS5JUV9MQVNUU0FMRVBSSUNFLjQ0MjIzAQAAABfbPAECAAAABjI3Mi4xNACeMokR/WTbCMXtSmX9ZNsIHUNJUS5IRC5JUV9MQVNUU0FMRVBSSUNFLjQzOTE0AQAAAJdABAACAAAABjE4NC43MgCeMokR/WTbCBFoSmX9ZNsIHkNJUS5KUE0uSVFfTEFTVFNBTEVQUklDRS40NDI0OQEAAABYDQoAAgAAAAYxNDkuNDEAnjKJEf1k2whgn0pl/WTbCB5DSVEuSk5KLklRX0xBU1RTQUxFUFJJQ0UuNDQyNDgBAAAAnSECAAIAAAAGMTYyLjk4AJ4yiRH9ZNsI1BFKZf1k2wgeQ0lRLkxMWS5JUV9MQVNUU0FMRVBSSUNFLjQ0MjQzAQAAABtbBAACAAAABjIwNS43NgCeMokR/WTbCIJASmX9ZNsIH0NJUS5OVkRBLklRX0xBU1RTQUxFUFJJQ0UuNDM4ODABAAAAM34AAAIAAAAGNzguNjc1AJ4yiRH9ZNsIeOpJZf1k2wgfQ0lRLlRTTEEuSVFfTEFTVFNBTEVQUklDRS40NDIzNAEAAAAQxqIBAgAAAAoyODQuMDc2NjY2AJ4yiRH9ZNsIeOpJZf1k2wgdQ0lRLlBHLklRX0xBU1RTQUxFUFJJQ0UuNDQwNTIBAAAAMIIAAAIAAAAGMTMzLjU1AJ4yiRH9ZNsIY5tJZf1k2wgeQ0lRLlhPTS5JUV9MQVNU</t>
-  </si>
-  <si>
-    <t>U0FMRVBSSUNFLjQ0MjUwAQAAAEIzBgACAAAABTU1LjA1AJ4yiRH9ZNsI0sJJZf1k2wgeQ0lRLlBGRS5JUV9MQVNUU0FMRVBSSUNFLjQ0MjUxAQAAAN55AgACAAAABTMzLjc1AJ4yiRH9ZNsI0UhJZf1k2wgcQ0lRLlYuSVFfTEFTVFNBTEVQUklDRS40NDE1MwEAAABLf0QCAgAAAAYyMDcuODMAnjKJEf1k2wgMdEll/WTbCB5DSVEuUEVQLklRX0xBU1RTQUxFUFJJQ0UuNDQyMzcBAAAAVoAAAAIAAAAFMTM3LjcAnjKJEf1k2wgH9Uhl/WTbCB5DSVEuVU5ILklRX0xBU1RTQUxFUFJJQ0UuNDQyNTUBAAAA4ZgBAAIAAAAGMzMyLjIyAJ4yiRH9ZNsIiSxJZf1k2wgfQ0lRLkFBUEwuSVFfTEFTVFNBTEVQUklDRS40NDUwNQEAAABpYQAAAgAAAAYxNTEuMjgAwzkmFf1k2wgabMOj/WTbCB5DSVEuQ1ZYLklRX0xBU1RTQUxFUFJJQ0UuNDQ2MjMBAAAAyoABAAIAAAAGMTU2LjIyAMM5JhX9ZNsIGmzDo/1k2wgeQ0lRLkJSSy5JUV9MQVNUU0FMRVBSSUNFLjQ0MTA3AQAAAB/STAECAAAABjE2LjYyNQDDOSYV/WTbCGBYw6P9ZNsIHkNJUS5BQlQuSVFfTEFTVFNBTEVQUklDRS40NDYxNwEAAAC7xgMAAgAAAAYxMjIuNDEAwzkmFf1k2whgWMOj/WTbCB9DSVEuQU1aTi5JUV9MQVNUU0FMRVBSSUNFLjQ0NjAzAQAAAD1JAAACAAAACDE1My4yOTM1AMM5JhX9ZNsIxDDDo/1k2wgfQ0lRLkFCQlYuSVFfTEFTVFNBTEVQUklDRS40</t>
-  </si>
-  <si>
-    <t>NDYxNwEAAAAKAXUIAgAAAAYxNDkuNTQAwzkmFf1k2wink8Oj/WTbCB9DSVEuQVZHTy5JUV9MQVNUU0FMRVBSSUNFLjQ0NTU0AQAAAPC2fQECAAAABTY2NC44AMM5JhX9ZNsIp5PDo/1k2wgfQ0lRLkNPU1QuSVFfTEFTVFNBTEVQUklDRS40NDQ4MgEAAACRagEAAgAAAAU0NDUuMwDDOSYV/WTbCBpsw6P9ZNsIH0NJUS5HT09HLklRX0xBU1RTQUxFUFJJQ0UuNDQ2MDEBAAAAqHEAAAIAAAAHMTQxLjQ1MwDDOSYV/WTbCBpsw6P9ZNsIHkNJUS5CQUMuSVFfTEFTVFNBTEVQUklDRS40NDYyMQEAAABpSgAAAgAAAAU0Mi40NwDDOSYV/WTbCBpsw6P9ZNsIHkNJUS5NUksuSVFfTEFTVFNBTEVQUklDRS40NDYyNAEAAAD2ZgQAAgAAAAU3Ny44MwDDOSYV/WTbCGBYw6P9ZNsIH0NJUS5NU0ZULklRX0xBU1RTQUxFUFJJQ0UuNDQ0MTMBAAAAS1UAAAIAAAAGMjg5LjUyAMM5JhX9ZNsIxDDDo/1k2wgdQ0lRLktPLklRX0xBU1RTQUxFUFJJQ0UuNDQ2MjEBAAAAEmgAAAIAAAAFNjEuOTcAwzkmFf1k2wjEMMOj/WTbCB5DSVEuTUNELklRX0xBU1RTQUxFUFJJQ0UuNDQ2MjMBAAAA4CACAAIAAAAGMjM2LjY1AMM5JhX9ZNsIp5PDo/1k2wgfQ0lRLk1FVEEuSVFfTEFTVFNBTEVQUklDRS40NDYwMgEAAAAX2zwBAgAAAAYyMjguMDcAL1YmFf1k2wink8Oj/WTbCB1DSVEuSEQuSVFfTEFTVFNBTEVQUklDRS40NDI4NgEAAACXQAQA</t>
-  </si>
-  <si>
-    <t>AgAAAAYzMDUuMjUAL1YmFf1k2wgabMOj/WTbCB5DSVEuSlBNLklRX0xBU1RTQUxFUFJJQ0UuNDQ2MjEBAAAAWA0KAAIAAAAGMTM2LjQ1AC9WJhX9ZNsIGmzDo/1k2wgeQ0lRLkpOSi5JUV9MQVNUU0FMRVBSSUNFLjQ0NjE2AQAAAJ0hAgACAAAABjE1OC4xNAAvViYV/WTbCBpsw6P9ZNsIHkNJUS5MTFkuSVFfTEFTVFNBTEVQUklDRS40NDYyMgEAAAAbWwQAAgAAAAYyNTQuMTcAL1YmFf1k2whgWMOj/WTbCB9DSVEuTlZEQS5JUV9MQVNUU0FMRVBSSUNFLjQ0MjYwAQAAADN+AAACAAAABzEyNC42MTUAL1YmFf1k2wjEMMOj/WTbCB9DSVEuVFNMQS5JUV9MQVNUU0FMRVBSSUNFLjQ0NjA2AQAAABDGogECAAAABjI5MS45MgAvViYV/WTbCMQww6P9ZNsIHUNJUS5QRy5JUV9MQVNUU0FMRVBSSUNFLjQ0NDIxAQAAADCCAAACAAAABjE0My42NAAvViYV/WTbCKeTw6P9ZNsIHkNJUS5YT00uSVFfTEFTVFNBTEVQUklDRS40NDYyMgEAAABCMwYAAgAAAAU4MC41MwAvViYV/WTbCBpsw6P9ZNsIHkNJUS5QRkUuSVFfTEFTVFNBTEVQUklDRS40NDYyMwEAAADeeQIAAgAAAAU0Ny44MwAvViYV/WTbCBpsw6P9ZNsIHENJUS5WLklRX0xBU1RTQUxFUFJJQ0UuNDQ1MjUBAAAAS39EAgIAAAAGMjAzLjI1AC9WJhX9ZNsIGmzDo/1k2wgeQ0lRLlBFUC5JUV9MQVNUU0FMRVBSSUNFLjQ0NjA5AQAAAFaAAAACAAAABjE2Ni43NQAv</t>
-  </si>
-  <si>
-    <t>ViYV/WTbCBpsw6P9ZNsIHkNJUS5VTkguSVFfTEFTVFNBTEVQUklDRS40NDYxNAEAAADhmAEAAgAAAAY0NjIuNTEAL1YmFf1k2whgWMOj/WTbCB5DSVEuVE1PLklRX0xBU1RTQUxFUFJJQ0UuNDQ2MjMBAAAA/3oBAAIAAAAGNTU0LjI5AC9WJhX9ZNsIxDDDo/1k2wgeQ0lRLldNVC5JUV9MQVNUU0FMRVBSSUNFLjQ0MjgxAQAAAN/GBAACAAAABjEzNS4xMwAvViYV/WTbCMQww6P9ZNsIH0NJUS5BQVBMLklRX0xBU1RTQUxFUFJJQ0UuNDQxNDEBAAAAaWEAAAIAAAAGMTE4LjY5AN0GYjf9ZNsIEZNMZf1k2wgeQ0lRLkNWWC5JUV9MQVNUU0FMRVBSSUNFLjQ0MjU5AQAAAMqAAQACAAAABTEwNC41AN0GYjf9ZNsI77pMZf1k2wgeQ0lRLkJSSy5JUV9MQVNUU0FMRVBSSUNFLjQzNzQzAQAAAB/STAECAAAAAjIwAN0GYjf9ZNsI77pMZf1k2wgeQ0lRLkFCVC5JUV9MQVNUU0FMRVBSSUNFLjQ0MjUzAQAAALvGAwACAAAABjExOS43OADdBmI3/WTbCPYmTGX9ZNsIH0NJUS5BTVpOLklRX0xBU1RTQUxFUFJJQ0UuNDQyMzcBAAAAPUkAAAIAAAAHMTY0LjMyOQDdBmI3/WTbCLpWTGX9ZNsIH0NJUS5BQkJWLklRX0xBU1RTQUxFUFJJQ0UuNDQyNTMBAAAACgF1CAIAAAAGMTA3Ljc0AN0GYjf9ZNsIiP9LZf1k2wgfQ0lRLkFWR08uSVFfTEFTVFNBTEVQUklDRS40NDE5MAEAAADwtn0BAgAAAAY0MzEuNDYA3QZiN/1k2wj2Jkxl</t>
-  </si>
-  <si>
-    <t>/WTbCB9DSVEuQ09TVC5JUV9MQVNUU0FMRVBSSUNFLjQ0MTE4AQAAAJFqAQACAAAABjM3OC4zNADdBmI3/WTbCF+oS2X9ZNsIH0NJUS5HT09HLklRX0xBU1RTQUxFUFJJQ0UuNDQyMzcBAAAAqHEAAAIAAAAHMTA0Ljc2OQDdBmI3/WTbCHzPS2X9ZNsIHkNJUS5CQUMuSVFfTEFTVFNBTEVQUklDRS40NDI1OAEAAABpSgAAAgAAAAUzNi40MgDdBmI3/WTbCChUS2X9ZNsIHkNJUS5NUksuSVFfTEFTVFNBTEVQUklDRS40NDI1OQEAAAD2ZgQAAgAAAAU3Mi4xNwDdBmI3/WTbCBOBS2X9ZNsIH0NJUS5NU0ZULklRX0xBU1RTQUxFUFJJQ0UuNDQwNTABAAAAS1UAAAIAAAAGMjEyLjQ4AN0GYjf9ZNsIgQFLZf1k2wgdQ0lRLktPLklRX0xBU1RTQUxFUFJJQ0UuNDQyNTkBAAAAEmgAAAIAAAAFNDkuOTQA3QZiN/1k2wjOKEtl/WTbCB5DSVEuTUNELklRX0xBU1RTQUxFUFJJQ0UuNDQyNTcBAAAA4CACAAIAAAAGMjA4LjY3AN0GYjf9ZNsI28ZKZf1k2wgfQ0lRLk1FVEEuSVFfTEFTVFNBTEVQUklDRS40NDIzMQEAAAAX2zwBAgAAAAYyNjYuNDkA3QZiN/1k2wjF7Upl/WTbCB1DSVEuSEQuSVFfTEFTVFNBTEVQUklDRS40MzkyMgEAAACXQAQAAgAAAAYxNzguNjMA3QZiN/1k2wgRaEpl/WTbCB5DSVEuSlBNLklRX0xBU1RTQUxFUFJJQ0UuNDQyNTcBAAAAWA0KAAIAAAAGMTUwLjAxAN0GYjf9ZNsIYJ9KZf1k2wgeQ0lRLkpO</t>
-  </si>
-  <si>
-    <t>Si5JUV9MQVNUU0FMRVBSSUNFLjQ0MjU2AQAAAJ0hAgACAAAABjE1OS4zMgDdBmI3/WTbCNQRSmX9ZNsIHkNJUS5MTFkuSVFfTEFTVFNBTEVQUklDRS40NDI1MQEAAAAbWwQAAgAAAAYyMDQuNTIA3QZiN/1k2wgRaEpl/WTbCB9DSVEuTlZEQS5JUV9MQVNUU0FMRVBSSUNFLjQzODg4AQAAADN+AAACAAAABTYzLjE1AN0GYjf9ZNsIeOpJZf1k2wgfQ0lRLlRTTEEuSVFfTEFTVFNBTEVQUklDRS40NDI0MgEAAAAQxqIBAgAAAAYyNzIuMDQA3QZiN/1k2wjUEUpl/WTbCB1DSVEuUEcuSVFfTEFTVFNBTEVQUklDRS40NDA2MAEAAAAwggAAAgAAAAUxMzUuNQDdBmI3/WTbCGObSWX9ZNsIHkNJUS5YT00uSVFfTEFTVFNBTEVQUklDRS40NDI1OAEAAABCMwYAAgAAAAU1Ni41MgDdBmI3/WTbCNLCSWX9ZNsIHkNJUS5QRkUuSVFfTEFTVFNBTEVQUklDRS40NDI1OQEAAADeeQIAAgAAAAQzNC4yAN0GYjf9ZNsI0UhJZf1k2wgcQ0lRLlYuSVFfTEFTVFNBTEVQUklDRS40NDE2MQEAAABLf0QCAgAAAAYyMTAuODkA3QZiN/1k2wgMdEll/WTbCB5DSVEuUEVQLklRX0xBU1RTQUxFUFJJQ0UuNDQyNDUBAAAAVoAAAAIAAAAGMTM1LjM3AN0GYjf9ZNsIB/VIZf1k2wgeQ0lRLlVOSC5JUV9MQVNUU0FMRVBSSUNFLjQ0MjYzAQAAAOGYAQACAAAABjM1MC4xNwDdBmI3/WTbCIksSWX9ZNsIH0NJUS5BQVBMLklRX0xBU1RTQUxFUFJJ</t>
-  </si>
-  <si>
-    <t>Q0UuNDQ0OTcBAAAAaWEAAAIAAAAGMTUyLjU3AKnPWpj9ZNsISe5zmP1k2wgeQ0lRLkNWWC5JUV9MQVNUU0FMRVBSSUNFLjQ0NjE1AQAAAMqAAQACAAAABjEzNS41NQCr/Qed/WTbCKOpI539ZNsIHkNJUS5CUksuSVFfTEFTVFNBTEVQUklDRS40NDA5OQEAAAAf0kwBAgAAAAYxNi43NzUAq/0Hnf1k2wijqSOd/WTbCB5DSVEuQUJULklRX0xBU1RTQUxFUFJJQ0UuNDQ2MDkBAAAAu8YDAAIAAAAGMTIwLjU4AKv9B539ZNsIo6kjnf1k2wgfQ0lRLkFNWk4uSVFfTEFTVFNBTEVQUklDRS40NDU5NQEAAAA9SQAAAgAAAAgxMzguODQ1NQCr/Qed/WTbCKOpI539ZNsIH0NJUS5BQkJWLklRX0xBU1RTQUxFUFJJQ0UuNDQ2MDkBAAAACgF1CAIAAAAGMTQ0Ljk3AKv9B539ZNsIo6kjnf1k2wgfQ0lRLkFWR08uSVFfTEFTVFNBTEVQUklDRS40NDU0NgEAAADwtn0BAgAAAAY2MjAuNjgAq/0Hnf1k2wijqSOd/WTbCB9DSVEuQ09TVC5JUV9MQVNUU0FMRVBSSUNFLjQ0NDc0AQAAAJFqAQACAAAABjQ0Ni4yNACr/Qed/WTbCKOpI539ZNsIH0NJUS5HT09HLklRX0xBU1RTQUxFUFJJQ0UuNDQ1OTMBAAAAqHEAAAIAAAAIMTM3Ljg3ODUAq/0Hnf1k2widgiOd/WTbCB5DSVEuQkFDLklRX0xBU1RTQUxFUFJJQ0UuNDQ2MTMBAAAAaUoAAAIAAAAFNDUuOTYAq/0Hnf1k2widgiOd/WTbCB5DSVEuTVJLLklRX0xBU1RTQUxFUFJJQ0Uu</t>
-  </si>
-  <si>
-    <t>NDQ2MTYBAAAA9mYEAAIAAAAFNzMuNTEAq/0Hnf1k2widgiOd/WTbCB9DSVEuTVNGVC5JUV9MQVNUU0FMRVBSSUNFLjQ0NDA1AQAAAEtVAAACAAAABjI4Ni4yMgCr/Qed/WTbCJ2CI539ZNsIHUNJUS5LTy5JUV9MQVNUU0FMRVBSSUNFLjQ0NjEzAQAAABJoAAACAAAABTYyLjU0AKv9B539ZNsInYIjnf1k2wgeQ0lRLk1DRC5JUV9MQVNUU0FMRVBSSUNFLjQ0NjE1AQAAAOAgAgACAAAABjI0Ny43OQCr/Qed/WTbCJ2CI539ZNsIH0NJUS5NRVRBLklRX0xBU1RTQUxFUFJJQ0UuNDQ1OTQBAAAAF9s8AQIAAAADMzIzAKv9B539ZNsIOVsjnf1k2wgdQ0lRLkhELklRX0xBU1RTQUxFUFJJQ0UuNDQyNzgBAAAAl0AEAAIAAAAGMjg5Ljk4AKv9B539ZNsIOVsjnf1k2wgeQ0lRLkpQTS5JUV9MQVNUU0FMRVBSSUNFLjQ0NjEzAQAAAFgNCgACAAAABjE1Mi4xNACr/Qed/WTbCDlbI539ZNsIHkNJUS5KTkouSVFfTEFTVFNBTEVQUklDRS40NDYwOAEAAACdIQIAAgAAAAYxNjcuMjEAq/0Hnf1k2wg5WyOd/WTbCB5DSVEuTExZLklRX0xBU1RTQUxFUFJJQ0UuNDQ2MTQBAAAAG1sEAAIAAAAGMjM5LjEzAKv9B539ZNsInYIjnf1k2wgfQ0lRLk5WREEuSVFfTEFTVFNBTEVQUklDRS40NDI1MgEAAAAzfgAAAgAAAAcxMzMuMDc1AKv9B539ZNsInYIjnf1k2wgfQ0lRLlRTTEEuSVFfTEFTVFNBTEVQUklDRS40NDU5OAEAAAAQxqIB</t>
-  </si>
-  <si>
-    <t>AgAAAAozMDcuNzczMzMzAKv9B539ZNsI+SYjnf1k2wgdQ0lRLlBHLklRX0xBU1RTQUxFUFJJQ0UuNDQ0MTMBAAAAMIIAAAIAAAAFMTQyLjUAq/0Hnf1k2wj5JiOd/WTbCB5DSVEuWE9NLklRX0xBU1RTQUxFUFJJQ0UuNDQ2MTQBAAAAQjMGAAIAAAAFNzYuNDYAq/0Hnf1k2wj5JiOd/WTbCB5DSVEuUEZFLklRX0xBU1RTQUxFUFJJQ0UuNDQ2MTUBAAAA3nkCAAIAAAAFNDYuODcAq/0Hnf1k2wj5JiOd/WTbCBxDSVEuVi5JUV9MQVNUU0FMRVBSSUNFLjQ0NTE3AQAAAEt/RAICAAAABjIwNS4wNgCr/Qed/WTbCDlbI539ZNsIHkNJUS5QRVAuSVFfTEFTVFNBTEVQUklDRS40NDYwMQEAAABWgAAAAgAAAAYxNzEuOTQAq/0Hnf1k2wg5WyOd/WTbCB5DSVEuVU5ILklRX0xBU1RTQUxFUFJJQ0UuNDQ2MDYBAAAA4ZgBAAIAAAAFNDc0LjQAq/0Hnf1k2wjLACOd/WTbCB5DSVEuVE1PLklRX0xBU1RTQUxFUFJJQ0UuNDQ2MTUBAAAA/3oBAAIAAAAGNTI4LjU4AKv9B539ZNsIywAjnf1k2wgeQ0lRLldNVC5JUV9MQVNUU0FMRVBSSUNFLjQ0MjczAQAAAN/GBAACAAAABjEzMC4wMQCr/Qed/WTbCPkmI539ZNsIH0NJUS5BQVBMLklRX0xBU1RTQUxFUFJJQ0UuNDQ4NjEBAAAAaWEAAAIAAAAFMTQ0LjgAx9SyvP1k2wj5Z828/WTbCB5DSVEuQ1ZYLklRX0xBU1RTQUxFUFJJQ0UuNDQ5NzkBAAAAyoABAAIAAAAGMTYwLjM1AMfU</t>
-  </si>
-  <si>
-    <t>srz9ZNsI+WfNvP1k2wgeQ0lRLkJSSy5JUV9MQVNUU0FMRVBSSUNFLjQ0NDY1AQAAAB/STAECAAAABTIzLjc1AMfUsrz9ZNsITpfNvP1k2wgeQ0lRLkFCVC5JUV9MQVNUU0FMRVBSSUNFLjQ0OTczAQAAALvGAwACAAAABjEwNi4wOADH1LK8/WTbCE6Xzbz9ZNsIH0NJUS5BTVpOLklRX0xBU1RTQUxFUFJJQ0UuNDQ5NTkBAAAAPUkAAAIAAAAGMTEyLjkxAMfUsrz9ZNsITpfNvP1k2wgfQ0lRLkFCQlYuSVFfTEFTVFNBTEVQUklDRS40NDk3MwEAAAAKAXUIAgAAAAYxNDkuNTMAx9SyvP1k2whOl828/WTbCB9DSVEuQVZHTy5JUV9MQVNUU0FMRVBSSUNFLjQ0OTEwAQAAAPC2fQECAAAAAzU1OADH1LK8/WTbCA2rzbz9ZNsIH0NJUS5DT1NULklRX0xBU1RTQUxFUFJJQ0UuNDQ4MzgBAAAAkWoBAAIAAAAGNDg2LjEzAMfUsrz9ZNsI+WfNvP1k2wgfQ0lRLkdPT0cuSVFfTEFTVFNBTEVQUklDRS40NDk1OQEAAACocQAAAgAAAAUxMDguOADH1LK8/WTbCPlnzbz9ZNsIHkNJUS5CQUMuSVFfTEFTVFNBTEVQUklDRS40NDk3OAEAAABpSgAAAgAAAAUzNC41MgDH1LK8/WTbCPlnzbz9ZNsIHkNJUS5NUksuSVFfTEFTVFNBTEVQUklDRS40NDk4MAEAAAD2ZgQAAgAAAAYxMTAuNTkAx9SyvP1k2wj5Z828/WTbCB9DSVEuTVNGVC5JUV9MQVNUU0FMRVBSSUNFLjQ0NzY5AQAAAEtVAAACAAAABjI2OC43NADH1LK8/WTbCPlnzbz9</t>
-  </si>
-  <si>
-    <t>ZNsIHUNJUS5LTy5JUV9MQVNUU0FMRVBSSUNFLjQ0OTc3AQAAABJoAAACAAAABTYwLjEyAMfUsrz9ZNsI+WfNvP1k2wgeQ0lRLk1DRC5JUV9MQVNUU0FMRVBSSUNFLjQ0OTgwAQAAAOAgAgACAAAABjI2Ni43OADH1LK8/WTbCKEyzbz9ZNsIH0NJUS5NRVRBLklRX0xBU1RTQUxFUFJJQ0UuNDQ5NTgBAAAAF9s8AQIAAAAGMTUzLjEyAMfUsrz9ZNsIoTLNvP1k2wgdQ0lRLkhELklRX0xBU1RTQUxFUFJJQ0UuNDQ2NDIBAAAAl0AEAAIAAAAGMzI5LjczAMfUsrz9ZNsIoTLNvP1k2wgeQ0lRLkpQTS5JUV9MQVNUU0FMRVBSSUNFLjQ0OTc3AQAAAFgNCgACAAAABjE0Mi4yNADH1LK8/WTbCKEyzbz9ZNsIHkNJUS5KTkouSVFfTEFTVFNBTEVQUklDRS40NDk3MgEAAACdIQIAAgAAAAYxNTkuMzcAx9SyvP1k2wihMs28/WTbCB5DSVEuTExZLklRX0xBU1RTQUxFUFJJQ0UuNDQ5NzgBAAAAG1sEAAIAAAAGMzI3LjUxAMfUsrz9ZNsI+WfNvP1k2wgfQ0lRLk5WREEuSVFfTEFTVFNBTEVQUklDRS40NDYzNwEAAAAzfgAAAgAAAAYyNDcuNjYAx9SyvP1k2wiYAM28/WTbCB9DSVEuVFNMQS5JUV9MQVNUU0FMRVBSSUNFLjQ0OTU2AQAAABDGogECAAAABjE2Ni42NgDH1LK8/WTbCJgAzbz9ZNsIHUNJUS5QRy5JUV9MQVNUU0FMRVBSSUNFLjQ0Nzc3AQAAADCCAAACAAAABjE0NC42NQDH1LK8/WTbCJgAzbz9ZNsIHkNJUS5YT00u</t>
-  </si>
-  <si>
-    <t>SVFfTEFTVFNBTEVQUklDRS40NDk3OAEAAABCMwYAAgAAAAYxMTEuMTcAx9SyvP1k2wihMs28/WTbCB5DSVEuUEZFLklRX0xBU1RTQUxFUFJJQ0UuNDQ5NzkBAAAA3nkCAAIAAAAFNDIuMzgAx9SyvP1k2wihMs28/WTbCBxDSVEuVi5JUV9MQVNUU0FMRVBSSUNFLjQ0ODgwAQAAAEt/RAICAAAABjIwOS45OQDH1LK8/WTbCKEyzbz9ZNsIHkNJUS5QRVAuSVFfTEFTVFNBTEVQUklDRS40NDk2NQEAAABWgAAAAgAAAAYxNzEuMTYAx9SyvP1k2wgt2cy8/WTbCB5DSVEuVU5ILklRX0xBU1RTQUxFUFJJQ0UuNDQ5ODABAAAA4ZgBAAIAAAAGNDkxLjY5AMfUsrz9ZNsImADNvP1k2wgeQ0lRLlRNTy5JUV9MQVNUU0FMRVBSSUNFLjQ0OTc5AQAAAP96AQACAAAABTU0OC40AMfUsrz9ZNsImADNvP1k2wgeQ0lRLldNVC5JUV9MQVNUU0FMRVBSSUNFLjQ0NjM3AQAAAN/GBAACAAAABjE0NS4wMQDH1LK8/WTbCJgAzbz9ZNsIH0NJUS5BQVBMLklRX0xBU1RTQUxFUFJJQ0UuNDQ4NjkBAAAAaWEAAAIAAAAGMTM4LjM4ACa8LsL9ZNsITGBMwv1k2wgeQ0lRLkNWWC5JUV9MQVNUU0FMRVBSSUNFLjQ0OTg3AQAAAMqAAQACAAAABjE2Mi41NgAmvC7C/WTbCPZzTML9ZNsIHkNJUS5CUksuSVFfTEFTVFNBTEVQUklDRS40NDQ3MwEAAAAf0kwBAgAAAAQyNS4xACa8LsL9ZNsI9nNMwv1k2wgeQ0lRLkFCVC5JUV9MQVNUU0FMRVBSSUNF</t>
-  </si>
-  <si>
-    <t>LjQ0OTgxAQAAALvGAwACAAAABjEwMC40NgAmvC7C/WTbCPZzTML9ZNsIH0NJUS5BTVpOLklRX0xBU1RTQUxFUFJJQ0UuNDQ5NjcBAAAAPUkAAAIAAAAFOTcuNjEAJrwuwv1k2wj2c0zC/WTbCB9DSVEuQUJCVi5JUV9MQVNUU0FMRVBSSUNFLjQ0OTgxAQAAAAoBdQgCAAAABjE1Mi43MQAmvC7C/WTbCPZzTML9ZNsIH0NJUS5BVkdPLklRX0xBU1RTQUxFUFJJQ0UuNDQ5MTgBAAAA8LZ9AQIAAAAGNTUyLjQzACa8LsL9ZNsI9nNMwv1k2wgfQ0lRLkNPU1QuSVFfTEFTVFNBTEVQUklDRS40NDg0NgEAAACRagEAAgAAAAY0NjYuMzgAJrwuwv1k2wiBOEzC/WTbCB9DSVEuR09PRy5JUV9MQVNUU0FMRVBSSUNFLjQ0OTY3AQAAAKhxAAACAAAABTk0Ljg2ACa8LsL9ZNsIgThMwv1k2wgeQ0lRLkJBQy5JUV9MQVNUU0FMRVBSSUNFLjQ0OTg2AQAAAGlKAAACAAAABTM0LjE0ACa8LsL9ZNsIgThMwv1k2wgeQ0lRLk1SSy5JUV9MQVNUU0FMRVBSSUNFLjQ0OTg4AQAAAPZmBAACAAAABjEwNi44OAAmvC7C/WTbCExgTML9ZNsIH0NJUS5NU0ZULklRX0xBU1RTQUxFUFJJQ0UuNDQ3NzcBAAAAS1UAAAIAAAAGMjgzLjY1ACa8LsL9ZNsITGBMwv1k2wgdQ0lRLktPLklRX0xBU1RTQUxFUFJJQ0UuNDQ5ODUBAAAAEmgAAAIAAAAFNTkuNTEAJrwuwv1k2whMYEzC/WTbCB5DSVEuTUNELklRX0xBU1RTQUxFUFJJQ0UuNDQ5ODgBAAAA</t>
-  </si>
-  <si>
-    <t>4CACAAIAAAAGMjY5LjA3ACa8LsL9ZNsIRAlMwv1k2wgfQ0lRLk1FVEEuSVFfTEFTVFNBTEVQUklDRS40NDk2NgEAAAAX2zwBAgAAAAYxNzcuOTIAJrwuwv1k2whECUzC/WTbCB1DSVEuSEQuSVFfTEFTVFNBTEVQUklDRS40NDY1MAEAAACXQAQAAgAAAAYzMDguNDYAJrwuwv1k2wiBOEzC/WTbCB5DSVEuSlBNLklRX0xBU1RTQUxFUFJJQ0UuNDQ5ODUBAAAAWA0KAAIAAAAGMTQzLjM1ACa8LsL9ZNsIgThMwv1k2wgeQ0lRLkpOSi5JUV9MQVNUU0FMRVBSSUNFLjQ0OTgwAQAAAJ0hAgACAAAABjE1Ny43MwAmvC7C/WTbCIE4TML9ZNsIHkNJUS5MTFkuSVFfTEFTVFNBTEVQUklDRS40NDk4NgEAAAAbWwQAAgAAAAYzMTQuMTcAJrwuwv1k2wiBOEzC/WTbCB9DSVEuTlZEQS5JUV9MQVNUU0FMRVBSSUNFLjQ0NjQ1AQAAADN+AAACAAAABjI3Ni45MgAmvC7C/WTbCMTfS8L9ZNsIH0NJUS5UU0xBLklRX0xBU1RTQUxFUFJJQ0UuNDQ5NjQBAAAAEMaiAQIAAAAGMTk2LjgxACa8LsL9ZNsIRAlMwv1k2wgdQ0lRLlBHLklRX0xBU1RTQUxFUFJJQ0UuNDQ3ODUBAAAAMIIAAAIAAAAGMTQ2LjY3ACa8LsL9ZNsIRAlMwv1k2wgeQ0lRLlhPTS5JUV9MQVNUU0FMRVBSSUNFLjQ0OTg2AQAAAEIzBgACAAAABjExMC44OQAmvC7C/WTbCEQJTML9ZNsIHkNJUS5QRkUuSVFfTEFTVFNBTEVQUklDRS40NDk4NwEAAADeeQIAAgAAAAU0</t>
-  </si>
-  <si>
-    <t>MC42MgAmvC7C/WTbCEQJTML9ZNsIHENJUS5WLklRX0xBU1RTQUxFUFJJQ0UuNDQ4ODgBAAAAS39EAgIAAAAGMjExLjczACa8LsL9ZNsIRAlMwv1k2wgeQ0lRLlBFUC5JUV9MQVNUU0FMRVBSSUNFLjQ0OTczAQAAAFaAAAACAAAABjE3NS41MQAmvC7C/WTbCJm5S8L9ZNsIHkNJUS5VTkguSVFfTEFTVFNBTEVQUklDRS40NDk4OAEAAADhmAEAAgAAAAY0NzguNTYAJrwuwv1k2wiZuUvC/WTbCB5DSVEuVE1PLklRX0xBU1RTQUxFUFJJQ0UuNDQ5ODcBAAAA/3oBAAIAAAAGNTQ4Ljc1ACa8LsL9ZNsIxN9Lwv1k2wgeQ0lRLldNVC5JUV9MQVNUU0FMRVBSSUNFLjQ0NjQ1AQAAAN/GBAACAAAABjE0My40NQAmvC7C/WTbCMTfS8L9ZNsI</t>
+    <t>Authors:</t>
+  </si>
+  <si>
+    <t>Arijeet Grewal (arijeet.s.grewal.23@dartmouth.edu)</t>
+  </si>
+  <si>
+    <t>Kevin King (kevin.m.king.24@dartmouth.edu)</t>
+  </si>
+  <si>
+    <t>Seamus O'Connell (seamus.c.o'connell.23@dartmouth.edu)</t>
+  </si>
+  <si>
+    <t>For the Dartmouth College course COSC72 Final Project</t>
+  </si>
+  <si>
+    <t>Description:</t>
+  </si>
+  <si>
+    <t>This excel file uses the Capital IQ plugin to pull in financial information regarding company stock return 7 days after the 2020, 2021, and 2022 10K filings were released</t>
+  </si>
+  <si>
+    <t>BAABTAVMT0NBTAFI/////wFQVwAAAB9DSVEuQUFQTC5JUV9MQVNUU0FMRVBSSUNFLjQ0NDk3AQAAAGlhAAACAAAABjE1Mi41NwCpz1qY/WTbCEnuc5j9ZNsIHkNJUS5DVlguSVFfTEFTVFNBTEVQUklDRS40NDYxNQEAAADKgAEAAgAAAAYxMzUuNTUAq/0Hnf1k2wijqSOd/WTbCB5DSVEuQlJLLklRX0xBU1RTQUxFUFJJQ0UuNDQwOTkBAAAAH9JMAQIAAAAGMTYuNzc1AKv9B539ZNsIo6kjnf1k2wgeQ0lRLkFCVC5JUV9MQVNUU0FMRVBSSUNFLjQ0NjA5AQAAALvGAwACAAAABjEyMC41OACr/Qed/WTbCKOpI539ZNsIH0NJUS5BTVpOLklRX0xBU1RTQUxFUFJJQ0UuNDQ1OTUBAAAAPUkAAAIAAAAIMTM4Ljg0NTUAq/0Hnf1k2wijqSOd/WTbCB9DSVEuQUJCVi5JUV9MQVNUU0FMRVBSSUNFLjQ0NjA5AQAAAAoBdQgCAAAABjE0NC45NwCr/Qed/WTbCKOpI539ZNsIH0NJUS5BVkdPLklRX0xBU1RTQUxFUFJJQ0UuNDQ1NDYBAAAA8LZ9AQIAAAAGNjIwLjY4AKv9B539ZNsIo6kjnf1k2wgfQ0lRLkNPU1QuSVFfTEFTVFNBTEVQUklDRS40NDQ3NAEAAACRagEAAgAAAAY0NDYuMjQAq/0Hnf1k2wijqSOd/WTbCB9DSVEuR09PRy5JUV9MQVNUU0FMRVBSSUNFLjQ0NTkzAQAAAKhxAAACAAAACDEzNy44Nzg1AKv9B539ZNsInYIjnf1k2wgeQ0lRLkJBQy5JUV9MQVNUU0FMRVBSSUNFLjQ0NjEzAQAAAGlKAAACAAAABTQ1</t>
+  </si>
+  <si>
+    <t>Ljk2AKv9B539ZNsInYIjnf1k2wgeQ0lRLk1SSy5JUV9MQVNUU0FMRVBSSUNFLjQ0NjE2AQAAAPZmBAACAAAABTczLjUxAKv9B539ZNsInYIjnf1k2wgfQ0lRLk1TRlQuSVFfTEFTVFNBTEVQUklDRS40NDQwNQEAAABLVQAAAgAAAAYyODYuMjIAq/0Hnf1k2widgiOd/WTbCB1DSVEuS08uSVFfTEFTVFNBTEVQUklDRS40NDYxMwEAAAASaAAAAgAAAAU2Mi41NACr/Qed/WTbCJ2CI539ZNsIHkNJUS5NQ0QuSVFfTEFTVFNBTEVQUklDRS40NDYxNQEAAADgIAIAAgAAAAYyNDcuNzkAq/0Hnf1k2widgiOd/WTbCB9DSVEuTUVUQS5JUV9MQVNUU0FMRVBSSUNFLjQ0NTk0AQAAABfbPAECAAAAAzMyMwCr/Qed/WTbCDlbI539ZNsIHUNJUS5IRC5JUV9MQVNUU0FMRVBSSUNFLjQ0Mjc4AQAAAJdABAACAAAABjI4OS45OACr/Qed/WTbCDlbI539ZNsIHkNJUS5KUE0uSVFfTEFTVFNBTEVQUklDRS40NDYxMwEAAABYDQoAAgAAAAYxNTIuMTQAq/0Hnf1k2wg5WyOd/WTbCB5DSVEuSk5KLklRX0xBU1RTQUxFUFJJQ0UuNDQ2MDgBAAAAnSECAAIAAAAGMTY3LjIxAKv9B539ZNsIOVsjnf1k2wgeQ0lRLkxMWS5JUV9MQVNUU0FMRVBSSUNFLjQ0NjE0AQAAABtbBAACAAAABjIzOS4xMwCr/Qed/WTbCJ2CI539ZNsIH0NJUS5OVkRBLklRX0xBU1RTQUxFUFJJQ0UuNDQyNTIBAAAAM34AAAIAAAAHMTMzLjA3NQCr/Qed/WTbCJ2C</t>
+  </si>
+  <si>
+    <t>I539ZNsIH0NJUS5UU0xBLklRX0xBU1RTQUxFUFJJQ0UuNDQ1OTgBAAAAEMaiAQIAAAAKMzA3Ljc3MzMzMwCr/Qed/WTbCPkmI539ZNsIHUNJUS5QRy5JUV9MQVNUU0FMRVBSSUNFLjQ0NDEzAQAAADCCAAACAAAABTE0Mi41AKv9B539ZNsI+SYjnf1k2wgeQ0lRLlhPTS5JUV9MQVNUU0FMRVBSSUNFLjQ0NjE0AQAAAEIzBgACAAAABTc2LjQ2AKv9B539ZNsI+SYjnf1k2wgeQ0lRLlBGRS5JUV9MQVNUU0FMRVBSSUNFLjQ0NjE1AQAAAN55AgACAAAABTQ2Ljg3AKv9B539ZNsI+SYjnf1k2wgcQ0lRLlYuSVFfTEFTVFNBTEVQUklDRS40NDUxNwEAAABLf0QCAgAAAAYyMDUuMDYAq/0Hnf1k2wg5WyOd/WTbCB5DSVEuUEVQLklRX0xBU1RTQUxFUFJJQ0UuNDQ2MDEBAAAAVoAAAAIAAAAGMTcxLjk0AKv9B539ZNsIOVsjnf1k2wgeQ0lRLlVOSC5JUV9MQVNUU0FMRVBSSUNFLjQ0NjA2AQAAAOGYAQACAAAABTQ3NC40AKv9B539ZNsIywAjnf1k2wgeQ0lRLlRNTy5JUV9MQVNUU0FMRVBSSUNFLjQ0NjE1AQAAAP96AQACAAAABjUyOC41OACr/Qed/WTbCMsAI539ZNsIHkNJUS5XTVQuSVFfTEFTVFNBTEVQUklDRS40NDI3MwEAAADfxgQAAgAAAAYxMzAuMDEAq/0Hnf1k2wj5JiOd/WTbCB9DSVEuQUFQTC5JUV9MQVNUU0FMRVBSSUNFLjQ0ODYxAQAAAGlhAAACAAAABTE0NC44AMfUsrz9ZNsI+WfNvP1k2wgeQ0lRLkNW</t>
+  </si>
+  <si>
+    <t>WC5JUV9MQVNUU0FMRVBSSUNFLjQ0OTc5AQAAAMqAAQACAAAABjE2MC4zNQDH1LK8/WTbCPlnzbz9ZNsIHkNJUS5CUksuSVFfTEFTVFNBTEVQUklDRS40NDQ2NQEAAAAf0kwBAgAAAAUyMy43NQDH1LK8/WTbCE6Xzbz9ZNsIHkNJUS5BQlQuSVFfTEFTVFNBTEVQUklDRS40NDk3MwEAAAC7xgMAAgAAAAYxMDYuMDgAx9SyvP1k2whOl828/WTbCB9DSVEuQU1aTi5JUV9MQVNUU0FMRVBSSUNFLjQ0OTU5AQAAAD1JAAACAAAABjExMi45MQDH1LK8/WTbCE6Xzbz9ZNsIH0NJUS5BQkJWLklRX0xBU1RTQUxFUFJJQ0UuNDQ5NzMBAAAACgF1CAIAAAAGMTQ5LjUzAMfUsrz9ZNsITpfNvP1k2wgfQ0lRLkFWR08uSVFfTEFTVFNBTEVQUklDRS40NDkxMAEAAADwtn0BAgAAAAM1NTgAx9SyvP1k2wgNq828/WTbCB9DSVEuQ09TVC5JUV9MQVNUU0FMRVBSSUNFLjQ0ODM4AQAAAJFqAQACAAAABjQ4Ni4xMwDH1LK8/WTbCPlnzbz9ZNsIH0NJUS5HT09HLklRX0xBU1RTQUxFUFJJQ0UuNDQ5NTkBAAAAqHEAAAIAAAAFMTA4LjgAx9SyvP1k2wj5Z828/WTbCB5DSVEuQkFDLklRX0xBU1RTQUxFUFJJQ0UuNDQ5NzgBAAAAaUoAAAIAAAAFMzQuNTIAx9SyvP1k2wj5Z828/WTbCB5DSVEuTVJLLklRX0xBU1RTQUxFUFJJQ0UuNDQ5ODABAAAA9mYEAAIAAAAGMTEwLjU5AMfUsrz9ZNsI+WfNvP1k2wgfQ0lRLk1TRlQuSVFfTEFTVFNB</t>
+  </si>
+  <si>
+    <t>TEVQUklDRS40NDc2OQEAAABLVQAAAgAAAAYyNjguNzQAx9SyvP1k2wj5Z828/WTbCB1DSVEuS08uSVFfTEFTVFNBTEVQUklDRS40NDk3NwEAAAASaAAAAgAAAAU2MC4xMgDH1LK8/WTbCPlnzbz9ZNsIHkNJUS5NQ0QuSVFfTEFTVFNBTEVQUklDRS40NDk4MAEAAADgIAIAAgAAAAYyNjYuNzgAx9SyvP1k2wihMs28/WTbCB9DSVEuTUVUQS5JUV9MQVNUU0FMRVBSSUNFLjQ0OTU4AQAAABfbPAECAAAABjE1My4xMgDH1LK8/WTbCKEyzbz9ZNsIHUNJUS5IRC5JUV9MQVNUU0FMRVBSSUNFLjQ0NjQyAQAAAJdABAACAAAABjMyOS43MwDH1LK8/WTbCKEyzbz9ZNsIHkNJUS5KUE0uSVFfTEFTVFNBTEVQUklDRS40NDk3NwEAAABYDQoAAgAAAAYxNDIuMjQAx9SyvP1k2wihMs28/WTbCB5DSVEuSk5KLklRX0xBU1RTQUxFUFJJQ0UuNDQ5NzIBAAAAnSECAAIAAAAGMTU5LjM3AMfUsrz9ZNsIoTLNvP1k2wgeQ0lRLkxMWS5JUV9MQVNUU0FMRVBSSUNFLjQ0OTc4AQAAABtbBAACAAAABjMyNy41MQDH1LK8/WTbCPlnzbz9ZNsIH0NJUS5OVkRBLklRX0xBU1RTQUxFUFJJQ0UuNDQ2MzcBAAAAM34AAAIAAAAGMjQ3LjY2AMfUsrz9ZNsImADNvP1k2wgfQ0lRLlRTTEEuSVFfTEFTVFNBTEVQUklDRS40NDk1NgEAAAAQxqIBAgAAAAYxNjYuNjYAx9SyvP1k2wiYAM28/WTbCB1DSVEuUEcuSVFfTEFTVFNBTEVQUklDRS40NDc3</t>
+  </si>
+  <si>
+    <t>NwEAAAAwggAAAgAAAAYxNDQuNjUAx9SyvP1k2wiYAM28/WTbCB5DSVEuWE9NLklRX0xBU1RTQUxFUFJJQ0UuNDQ5NzgBAAAAQjMGAAIAAAAGMTExLjE3AMfUsrz9ZNsIoTLNvP1k2wgeQ0lRLlBGRS5JUV9MQVNUU0FMRVBSSUNFLjQ0OTc5AQAAAN55AgACAAAABTQyLjM4AMfUsrz9ZNsIoTLNvP1k2wgcQ0lRLlYuSVFfTEFTVFNBTEVQUklDRS40NDg4MAEAAABLf0QCAgAAAAYyMDkuOTkAx9SyvP1k2wihMs28/WTbCB5DSVEuUEVQLklRX0xBU1RTQUxFUFJJQ0UuNDQ5NjUBAAAAVoAAAAIAAAAGMTcxLjE2AMfUsrz9ZNsILdnMvP1k2wgeQ0lRLlVOSC5JUV9MQVNUU0FMRVBSSUNFLjQ0OTgwAQAAAOGYAQACAAAABjQ5MS42OQDH1LK8/WTbCJgAzbz9ZNsIHkNJUS5UTU8uSVFfTEFTVFNBTEVQUklDRS40NDk3OQEAAAD/egEAAgAAAAU1NDguNADH1LK8/WTbCJgAzbz9ZNsIHkNJUS5XTVQuSVFfTEFTVFNBTEVQUklDRS40NDYzNwEAAADfxgQAAgAAAAYxNDUuMDEAx9SyvP1k2wiYAM28/WTbCB9DSVEuQUFQTC5JUV9MQVNUU0FMRVBSSUNFLjQ0ODY5AQAAAGlhAAACAAAABjEzOC4zOAAmvC7C/WTbCExgTML9ZNsIHkNJUS5DVlguSVFfTEFTVFNBTEVQUklDRS40NDk4NwEAAADKgAEAAgAAAAYxNjIuNTYAJrwuwv1k2wj2c0zC/WTbCB5DSVEuQlJLLklRX0xBU1RTQUxFUFJJQ0UuNDQ0NzMBAAAAH9JMAQIAAAAE</t>
+  </si>
+  <si>
+    <t>MjUuMQAmvC7C/WTbCPZzTML9ZNsIHkNJUS5BQlQuSVFfTEFTVFNBTEVQUklDRS40NDk4MQEAAAC7xgMAAgAAAAYxMDAuNDYAJrwuwv1k2wj2c0zC/WTbCB9DSVEuQU1aTi5JUV9MQVNUU0FMRVBSSUNFLjQ0OTY3AQAAAD1JAAACAAAABTk3LjYxACa8LsL9ZNsI9nNMwv1k2wgfQ0lRLkFCQlYuSVFfTEFTVFNBTEVQUklDRS40NDk4MQEAAAAKAXUIAgAAAAYxNTIuNzEAJrwuwv1k2wj2c0zC/WTbCB9DSVEuQVZHTy5JUV9MQVNUU0FMRVBSSUNFLjQ0OTE4AQAAAPC2fQECAAAABjU1Mi40MwAmvC7C/WTbCPZzTML9ZNsIH0NJUS5DT1NULklRX0xBU1RTQUxFUFJJQ0UuNDQ4NDYBAAAAkWoBAAIAAAAGNDY2LjM4ACa8LsL9ZNsIgThMwv1k2wgfQ0lRLkdPT0cuSVFfTEFTVFNBTEVQUklDRS40NDk2NwEAAACocQAAAgAAAAU5NC44NgAmvC7C/WTbCIE4TML9ZNsIHkNJUS5CQUMuSVFfTEFTVFNBTEVQUklDRS40NDk4NgEAAABpSgAAAgAAAAUzNC4xNAAmvC7C/WTbCIE4TML9ZNsIHkNJUS5NUksuSVFfTEFTVFNBTEVQUklDRS40NDk4OAEAAAD2ZgQAAgAAAAYxMDYuODgAJrwuwv1k2whMYEzC/WTbCB9DSVEuTVNGVC5JUV9MQVNUU0FMRVBSSUNFLjQ0Nzc3AQAAAEtVAAACAAAABjI4My42NQAmvC7C/WTbCExgTML9ZNsIHUNJUS5LTy5JUV9MQVNUU0FMRVBSSUNFLjQ0OTg1AQAAABJoAAACAAAABTU5LjUxACa8LsL9</t>
+  </si>
+  <si>
+    <t>ZNsITGBMwv1k2wgeQ0lRLk1DRC5JUV9MQVNUU0FMRVBSSUNFLjQ0OTg4AQAAAOAgAgACAAAABjI2OS4wNwAmvC7C/WTbCEQJTML9ZNsIH0NJUS5NRVRBLklRX0xBU1RTQUxFUFJJQ0UuNDQ5NjYBAAAAF9s8AQIAAAAGMTc3LjkyACa8LsL9ZNsIRAlMwv1k2wgdQ0lRLkhELklRX0xBU1RTQUxFUFJJQ0UuNDQ2NTABAAAAl0AEAAIAAAAGMzA4LjQ2ACa8LsL9ZNsIgThMwv1k2wgeQ0lRLkpQTS5JUV9MQVNUU0FMRVBSSUNFLjQ0OTg1AQAAAFgNCgACAAAABjE0My4zNQAmvC7C/WTbCIE4TML9ZNsIHkNJUS5KTkouSVFfTEFTVFNBTEVQUklDRS40NDk4MAEAAACdIQIAAgAAAAYxNTcuNzMAJrwuwv1k2wiBOEzC/WTbCB5DSVEuTExZLklRX0xBU1RTQUxFUFJJQ0UuNDQ5ODYBAAAAG1sEAAIAAAAGMzE0LjE3ACa8LsL9ZNsIgThMwv1k2wgfQ0lRLk5WREEuSVFfTEFTVFNBTEVQUklDRS40NDY0NQEAAAAzfgAAAgAAAAYyNzYuOTIAJrwuwv1k2wjE30vC/WTbCB9DSVEuVFNMQS5JUV9MQVNUU0FMRVBSSUNFLjQ0OTY0AQAAABDGogECAAAABjE5Ni44MQAmvC7C/WTbCEQJTML9ZNsIHUNJUS5QRy5JUV9MQVNUU0FMRVBSSUNFLjQ0Nzg1AQAAADCCAAACAAAABjE0Ni42NwAmvC7C/WTbCEQJTML9ZNsIHkNJUS5YT00uSVFfTEFTVFNBTEVQUklDRS40NDk4NgEAAABCMwYAAgAAAAYxMTAuODkAJrwuwv1k2whECUzC/WTb</t>
+  </si>
+  <si>
+    <t>CB5DSVEuUEZFLklRX0xBU1RTQUxFUFJJQ0UuNDQ5ODcBAAAA3nkCAAIAAAAFNDAuNjIAJrwuwv1k2whECUzC/WTbCBxDSVEuVi5JUV9MQVNUU0FMRVBSSUNFLjQ0ODg4AQAAAEt/RAICAAAABjIxMS43MwAmvC7C/WTbCEQJTML9ZNsIHkNJUS5QRVAuSVFfTEFTVFNBTEVQUklDRS40NDk3MwEAAABWgAAAAgAAAAYxNzUuNTEAJrwuwv1k2wiZuUvC/WTbCB5DSVEuVU5ILklRX0xBU1RTQUxFUFJJQ0UuNDQ5ODgBAAAA4ZgBAAIAAAAGNDc4LjU2ACa8LsL9ZNsImblLwv1k2wgeQ0lRLlRNTy5JUV9MQVNUU0FMRVBSSUNFLjQ0OTg3AQAAAP96AQACAAAABjU0OC43NQAmvC7C/WTbCMTfS8L9ZNsIHkNJUS5XTVQuSVFfTEFTVFNBTEVQUklDRS40NDY0NQEAAADfxgQAAgAAAAYxNDMuNDUAJrwuwv1k2wjE30vC/WTbCA==</t>
   </si>
 </sst>
 </file>
@@ -769,6 +710,102 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B471DD2D-A5C4-4FE6-85B6-49FB1F173C63}">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A1">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I1" t="s">
+        <v>72</v>
+      </c>
+      <c r="J1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5D9E38D-7D95-487F-BC6B-EA8766621A5F}">
+  <dimension ref="B2:C10"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.45">
+      <c r="C10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U33"/>
   <sheetViews>
@@ -3141,137 +3178,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2199F75-99E0-4DE0-BF2E-7403DAD53924}">
-  <dimension ref="A1:AK1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.45">
-      <c r="A1">
-        <v>37</v>
-      </c>
-      <c r="B1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I1" t="s">
-        <v>65</v>
-      </c>
-      <c r="J1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L1" t="s">
-        <v>68</v>
-      </c>
-      <c r="M1" t="s">
-        <v>69</v>
-      </c>
-      <c r="N1" t="s">
-        <v>70</v>
-      </c>
-      <c r="O1" t="s">
-        <v>71</v>
-      </c>
-      <c r="P1" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>73</v>
-      </c>
-      <c r="R1" t="s">
-        <v>74</v>
-      </c>
-      <c r="S1" t="s">
-        <v>75</v>
-      </c>
-      <c r="T1" t="s">
-        <v>76</v>
-      </c>
-      <c r="U1" t="s">
-        <v>77</v>
-      </c>
-      <c r="V1" t="s">
-        <v>78</v>
-      </c>
-      <c r="W1" t="s">
-        <v>79</v>
-      </c>
-      <c r="X1" t="s">
-        <v>80</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>82</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>83</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>84</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>85</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>86</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>87</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>88</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>89</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>90</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>91</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>92</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4C84066-4A0E-4955-B788-233E7FCD2F41}">
   <dimension ref="A2:D11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="101" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="101" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -3279,7 +3190,7 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -3287,7 +3198,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -3295,7 +3206,7 @@
     </row>
     <row r="4" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="8" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -3315,7 +3226,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B6" s="12">
         <v>23</v>
@@ -3329,7 +3240,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
@@ -3339,7 +3250,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -3349,7 +3260,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -3359,7 +3270,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -3369,7 +3280,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>

</xml_diff>